<commit_message>
Add raw hw files
</commit_message>
<xml_diff>
--- a/Hw_7/Problem4.xlsx
+++ b/Hw_7/Problem4.xlsx
@@ -322,11 +322,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="97844752"/>
-        <c:axId val="56386560"/>
+        <c:axId val="-640556288"/>
+        <c:axId val="-641001248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97844752"/>
+        <c:axId val="-640556288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -402,6 +402,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -438,12 +439,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56386560"/>
+        <c:crossAx val="-641001248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56386560"/>
+        <c:axId val="-641001248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -560,7 +561,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97844752"/>
+        <c:crossAx val="-640556288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1466,7 +1467,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>